<commit_message>
Update iter 3 test cases with protect
‘Protect’ test cases included in iter 3.
Update iter 6’s login test cases accordingly as well.
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 3/Iteration 3 Test Cases v2 result.xlsx
+++ b/Test Cases/Iteration 3/Iteration 3 Test Cases v2 result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="840" windowWidth="15540" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="9660" yWindow="460" windowWidth="15540" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>No</t>
   </si>
@@ -304,6 +304,43 @@
   </si>
   <si>
     <t xml:space="preserve">Account Not created and no message shown that account has been created. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protect </t>
+  </si>
+  <si>
+    <t>Unauthorise Access - Normal User Access Create User Page</t>
+  </si>
+  <si>
+    <t>Login with Test Case 7
+Email: ulinkassist_executive@hotmail.com 
+Password:  password!23
+Access directly : http://ec2-35-161-162-8.us-west-2.compute.amazonaws.com/U-Link/accountManagement.html</t>
+  </si>
+  <si>
+    <t>Page should direct to user home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unauthorise Access </t>
+  </si>
+  <si>
+    <t>Click the Logout button if it is login. 
+Access directly : http://ec2-35-161-162-8.us-west-2.compute.amazonaws.com/U-Link/index.html</t>
+  </si>
+  <si>
+    <t>Page should direct to login page</t>
+  </si>
+  <si>
+    <t>Click the Logout button if user is login. 
+Access directly : http://ec2-35-161-162-8.us-west-2.compute.amazonaws.com/U-Link/accountManagement.html</t>
+  </si>
+  <si>
+    <t>Click the Logout button if user is login. 
+Access directly : http://ec2-35-161-162-8.us-west-2.compute.amazonaws.com/U-Link/upload.html</t>
+  </si>
+  <si>
+    <t>Click the Logout button if user is login. 
+Access directly : http://ec2-35-161-162-8.us-west-2.compute.amazonaws.com/U-link/viewScreenings.html</t>
   </si>
 </sst>
 </file>
@@ -923,7 +960,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,60 +1428,110 @@
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+    <row r="25" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>

</xml_diff>